<commit_message>
Added Apache Commons Lang 2.4
</commit_message>
<xml_diff>
--- a/Canopy_Tasks_Ajmal/src/test/resources/excel/testdata.xlsx
+++ b/Canopy_Tasks_Ajmal/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AssignementCanopy\PageObjectwithFactories\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CanopyTasks\Canopy_Tasks_Ajmal\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,11 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="SignInTest" sheetId="1" r:id="rId1"/>
-    <sheet name="FlightSearchTest" sheetId="2" r:id="rId2"/>
+    <sheet name="Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Ajimulkhan - Personal View" guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Ajimulkhan - Personal View" guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Y</t>
   </si>
@@ -40,33 +40,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>Delhi, India (DEL-Indira Gandhi Intl.)</t>
-  </si>
-  <si>
-    <t>fromCity</t>
-  </si>
-  <si>
-    <t>toCity</t>
-  </si>
-  <si>
-    <t>Seattle, WA, United States (SEA-Seattle - Tacoma Intl.)</t>
-  </si>
-  <si>
-    <t>fromDate</t>
-  </si>
-  <si>
-    <t>toDate</t>
-  </si>
-  <si>
-    <t>14/12/2017</t>
-  </si>
-  <si>
-    <t>noOfAdults</t>
-  </si>
-  <si>
-    <t>noOfChildern</t>
   </si>
   <si>
     <t>TechGeek$123</t>
@@ -140,7 +113,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{677ACF80-ED14-49D9-8D0E-7F6384463936}" diskRevisions="1" revisionId="46" version="3">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5ACC00C2-7472-4ED6-AF0C-88E672E6C9F7}" diskRevisions="1" revisionId="61" version="5">
   <header guid="{D1219B9C-CFDB-4452-8E4B-2153DE6E93E9}" dateTime="2018-10-08T20:44:37" maxSheetId="3" userName="Ajimulkhan" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -154,6 +127,18 @@
     </sheetIdMap>
   </header>
   <header guid="{677ACF80-ED14-49D9-8D0E-7F6384463936}" dateTime="2018-10-09T13:25:00" maxSheetId="3" userName="Ajimulkhan" r:id="rId3" minRId="5" maxRId="46">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{EC994662-50F5-47A0-85E7-EDC47701242E}" dateTime="2018-10-12T23:36:51" maxSheetId="3" userName="Ajimulkhan" r:id="rId4" minRId="47" maxRId="61">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5ACC00C2-7472-4ED6-AF0C-88E672E6C9F7}" dateTime="2018-10-12T23:37:04" maxSheetId="3" userName="Ajimulkhan" r:id="rId5">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -421,6 +406,127 @@
       </nc>
     </rcc>
   </rrc>
+  <rcv guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" action="delete"/>
+  <rcv guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="47" sId="2">
+    <oc r="A1" t="inlineStr">
+      <is>
+        <t>fromCity</t>
+      </is>
+    </oc>
+    <nc r="A1"/>
+  </rcc>
+  <rcc rId="48" sId="2">
+    <oc r="B1" t="inlineStr">
+      <is>
+        <t>toCity</t>
+      </is>
+    </oc>
+    <nc r="B1"/>
+  </rcc>
+  <rcc rId="49" sId="2">
+    <oc r="C1" t="inlineStr">
+      <is>
+        <t>fromDate</t>
+      </is>
+    </oc>
+    <nc r="C1"/>
+  </rcc>
+  <rcc rId="50" sId="2">
+    <oc r="D1" t="inlineStr">
+      <is>
+        <t>toDate</t>
+      </is>
+    </oc>
+    <nc r="D1"/>
+  </rcc>
+  <rcc rId="51" sId="2">
+    <oc r="E1" t="inlineStr">
+      <is>
+        <t>noOfAdults</t>
+      </is>
+    </oc>
+    <nc r="E1"/>
+  </rcc>
+  <rcc rId="52" sId="2">
+    <oc r="F1" t="inlineStr">
+      <is>
+        <t>noOfChildern</t>
+      </is>
+    </oc>
+    <nc r="F1"/>
+  </rcc>
+  <rcc rId="53" sId="2">
+    <oc r="G1" t="inlineStr">
+      <is>
+        <t>runmode</t>
+      </is>
+    </oc>
+    <nc r="G1"/>
+  </rcc>
+  <rcc rId="54" sId="2">
+    <oc r="A2" t="inlineStr">
+      <is>
+        <t>Delhi, India (DEL-Indira Gandhi Intl.)</t>
+      </is>
+    </oc>
+    <nc r="A2"/>
+  </rcc>
+  <rcc rId="55" sId="2">
+    <oc r="B2" t="inlineStr">
+      <is>
+        <t>Seattle, WA, United States (SEA-Seattle - Tacoma Intl.)</t>
+      </is>
+    </oc>
+    <nc r="B2"/>
+  </rcc>
+  <rcc rId="56" sId="2" numFmtId="19">
+    <oc r="C2">
+      <v>43081</v>
+    </oc>
+    <nc r="C2"/>
+  </rcc>
+  <rcc rId="57" sId="2">
+    <oc r="D2" t="inlineStr">
+      <is>
+        <t>14/12/2017</t>
+      </is>
+    </oc>
+    <nc r="D2"/>
+  </rcc>
+  <rcc rId="58" sId="2">
+    <oc r="E2">
+      <v>2</v>
+    </oc>
+    <nc r="E2"/>
+  </rcc>
+  <rcc rId="59" sId="2">
+    <oc r="F2">
+      <v>2</v>
+    </oc>
+    <nc r="F2"/>
+  </rcc>
+  <rcc rId="60" sId="2">
+    <oc r="G2" t="inlineStr">
+      <is>
+        <t>Y</t>
+      </is>
+    </oc>
+    <nc r="G2"/>
+  </rcc>
+  <rcv guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" action="delete"/>
+  <rcv guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" action="add"/>
+  <rsnm rId="61" sheetId="2" oldName="[testdata.xlsx]FlightSearchTest" newName="[testdata.xlsx]Test"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" action="delete"/>
   <rcv guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}" action="add"/>
 </revisions>
@@ -698,12 +804,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -720,10 +826,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -732,7 +838,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -748,10 +854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H5" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,56 +865,13 @@
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43081</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6F3AD0DD-BF38-460E-97C4-DFDBACD74297}">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H5" sqref="A1:H5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>